<commit_message>
Generando rastreabilidad entre documentos analisis, matriz  y requerimientos
</commit_message>
<xml_diff>
--- a/Proyectos/ControlDeGastos/01. Requerimientos/ControlDeGastos-MatrizRastreabilidad.xlsx
+++ b/Proyectos/ControlDeGastos/01. Requerimientos/ControlDeGastos-MatrizRastreabilidad.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="43">
   <si>
     <t>Nombre del Proyecto:</t>
   </si>
@@ -89,6 +89,9 @@
     <t>CU13</t>
   </si>
   <si>
+    <t>CU14</t>
+  </si>
+  <si>
     <t>CRUD de Rubro</t>
   </si>
   <si>
@@ -135,6 +138,12 @@
   </si>
   <si>
     <t>Control de acceso de usuarios para evitar infiltración de usuarios no deseados</t>
+  </si>
+  <si>
+    <t>Interfaz loggin</t>
+  </si>
+  <si>
+    <t>Se pueden realizar traspasos entre cuentas </t>
   </si>
 </sst>
 </file>
@@ -283,7 +292,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -316,12 +325,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -330,6 +347,14 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -409,16 +434,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>640440</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>667800</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>79920</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>106560</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>823680</xdr:rowOff>
+      <xdr:rowOff>823320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -431,8 +456,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16286760" y="0"/>
-          <a:ext cx="3516840" cy="823680"/>
+          <a:off x="17152200" y="0"/>
+          <a:ext cx="3516120" cy="823320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -452,10 +477,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:36"/>
+  <dimension ref="1:31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -464,9 +489,11 @@
     <col collapsed="false" hidden="false" max="3" min="2" style="1" width="24.2793522267206"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4251012145749"/>
     <col collapsed="false" hidden="false" max="17" min="5" style="1" width="8.4251012145749"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="23"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="22.8502024291498"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="1" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="23"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="22.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1023" min="21" style="1" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1493,7 +1520,6 @@
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -1518,7 +1544,7 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
-      <c r="S2" s="0"/>
+      <c r="S2" s="4"/>
       <c r="T2" s="0"/>
       <c r="U2" s="0"/>
       <c r="V2" s="0"/>
@@ -2523,7 +2549,6 @@
       <c r="AMG2" s="0"/>
       <c r="AMH2" s="0"/>
       <c r="AMI2" s="0"/>
-      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -2548,7 +2573,7 @@
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="0"/>
+      <c r="S3" s="4"/>
       <c r="T3" s="0"/>
       <c r="U3" s="0"/>
       <c r="V3" s="0"/>
@@ -3553,7 +3578,6 @@
       <c r="AMG3" s="0"/>
       <c r="AMH3" s="0"/>
       <c r="AMI3" s="0"/>
-      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5"/>
@@ -3574,7 +3598,7 @@
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
-      <c r="S4" s="0"/>
+      <c r="S4" s="4"/>
       <c r="T4" s="0"/>
       <c r="U4" s="0"/>
       <c r="V4" s="0"/>
@@ -4579,7 +4603,6 @@
       <c r="AMG4" s="0"/>
       <c r="AMH4" s="0"/>
       <c r="AMI4" s="0"/>
-      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" s="7" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
@@ -4609,12 +4632,14 @@
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
-      <c r="R5" s="2" t="s">
+      <c r="R5" s="2"/>
+      <c r="S5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="T5" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6"/>
@@ -4660,118 +4685,124 @@
       <c r="Q6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="R6" s="2"/>
+      <c r="R6" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="n">
         <v>1</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="8" t="n">
+        <v>25</v>
+      </c>
+      <c r="C7" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="8" t="s">
+      <c r="D7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8" t="s">
+      <c r="E7" s="10" t="s">
         <v>27</v>
       </c>
+      <c r="F7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="n">
         <v>2</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="8" t="n">
+        <v>29</v>
+      </c>
+      <c r="C8" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8" t="s">
+      <c r="D8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8" t="s">
-        <v>29</v>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="n">
         <v>3</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="C9" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8" t="s">
+      <c r="D9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8" t="s">
-        <v>31</v>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4779,687 +4810,600 @@
         <v>4</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="8" t="n">
+        <v>33</v>
+      </c>
+      <c r="C10" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8" t="s">
+      <c r="D10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="O10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8" t="s">
-        <v>33</v>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="P10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="n">
+      <c r="A11" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="8" t="n">
+      <c r="B11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8" t="s">
+      <c r="D11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8" t="s">
-        <v>35</v>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="n">
+      <c r="A12" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="C12" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="8" t="n">
+      <c r="B13" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8" t="s">
+      <c r="D13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8" t="s">
-        <v>35</v>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="n">
+    <row r="14" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="n">
         <v>8</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="8" t="n">
-        <v>7</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8" t="s">
+      <c r="B14" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8" t="s">
-        <v>35</v>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="43.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="10" t="n">
+        <v>12</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8" t="s">
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="14" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="10" t="n">
+        <v>15</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="8"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="8"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
-      <c r="R34" s="8"/>
-      <c r="S34" s="8"/>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+      <c r="T31" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -5473,15 +5417,15 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:Q5"/>
-    <mergeCell ref="R5:R6"/>
     <mergeCell ref="S5:S6"/>
+    <mergeCell ref="T5:T6"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D7 D9 D11 D13 D15 D17 D19 D21 D23 D25 D27 D29 D31 D33 D35" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D7 D9 D11 D13 D16 D18 D20 D22 D24 D26 D28 D30" type="list">
       <formula1>"Activo,Concluido,Eliminado"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D8 D10 D12 D14 D16 D18 D20 D22 D24 D26 D28 D30 D32 D34 D36" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D8 D10 D12 D14:D15 D17 D19 D21 D23 D25 D27 D29 D31" type="list">
       <formula1>"Activo,Concluido,Eliminado,M-Activo,M-Concluido,M-Eliminado"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>